<commit_message>
File selection added in GUI, bugfixes and more
</commit_message>
<xml_diff>
--- a/documents/development/Active Tasklist.xlsx
+++ b/documents/development/Active Tasklist.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20372"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A01E770C-8B43-4933-9F5B-533665EDB613}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E06021D-7F0D-45EB-855A-A2134594CFD9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{4FAFD036-DF6C-46F8-9D4B-2736D29CB41D}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="28">
   <si>
     <t>☒</t>
   </si>
@@ -96,6 +96,15 @@
   </si>
   <si>
     <t>Investigate feasibility of GTK based UI for Linux and MacOS</t>
+  </si>
+  <si>
+    <t>Add possibility to load and display experimental Data in SEIRD model of GUI</t>
+  </si>
+  <si>
+    <t>Integrate Parameter Estimator into GUI</t>
+  </si>
+  <si>
+    <t>Parameter Estimator must be integrated into the GUI before the next meeting with Arne and Babett</t>
   </si>
 </sst>
 </file>
@@ -235,7 +244,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
@@ -275,6 +284,12 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="7" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -595,7 +610,7 @@
   <dimension ref="A1:H210"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="F14" sqref="F12:F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -629,8 +644,8 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
-        <v>1</v>
+      <c r="A2" s="8" t="s">
+        <v>0</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>9</v>
@@ -671,8 +686,8 @@
       </c>
     </row>
     <row r="4" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
-        <v>1</v>
+      <c r="A4" s="8" t="s">
+        <v>0</v>
       </c>
       <c r="B4" s="9" t="s">
         <v>8</v>
@@ -749,25 +764,47 @@
       </c>
       <c r="H7" s="13"/>
     </row>
-    <row r="8" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="10"/>
-      <c r="B8" s="11"/>
-      <c r="C8" s="12"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="12"/>
+    <row r="8" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A8" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="E8" s="15">
+        <v>44275</v>
+      </c>
       <c r="F8" s="12"/>
       <c r="G8">
         <v>7</v>
       </c>
       <c r="H8" s="13"/>
     </row>
-    <row r="9" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="10"/>
-      <c r="B9" s="11"/>
-      <c r="C9" s="12"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="12"/>
+    <row r="9" spans="1:8" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="E9" s="15">
+        <v>44279</v>
+      </c>
+      <c r="F9" s="12" t="s">
+        <v>27</v>
+      </c>
       <c r="G9">
         <v>8</v>
       </c>
@@ -2802,14 +2839,14 @@
       <c r="H210" s="13"/>
     </row>
   </sheetData>
-  <dataValidations xWindow="123" yWindow="284" count="1">
+  <dataValidations xWindow="146" yWindow="419" count="1">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Wrong" error="Invalid developer name" promptTitle="Developers" prompt="Select an available developer from the list" sqref="D1" xr:uid="{27FDAF98-F61C-482A-B10E-B03FAF805807}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xWindow="123" yWindow="284" count="3">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xWindow="146" yWindow="419" count="3">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Wrong" error="Invalid developer name" promptTitle="Developers" prompt="Select an available developer from the list" xr:uid="{F17BDB0B-530F-46D1-9A6E-3971E0C825C7}">
           <x14:formula1>
             <xm:f>Tabelle2!$A$2:$A$5</xm:f>

</xml_diff>

<commit_message>
Updated documentation and added function to automatically generate SEIRDs evaluate.lua
</commit_message>
<xml_diff>
--- a/documents/development/Active Tasklist.xlsx
+++ b/documents/development/Active Tasklist.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20372"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E06021D-7F0D-45EB-855A-A2134594CFD9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62004BFE-CDC7-4D9E-A641-12D21E141EF5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{4FAFD036-DF6C-46F8-9D4B-2736D29CB41D}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="30">
   <si>
     <t>☒</t>
   </si>
@@ -105,6 +105,12 @@
   </si>
   <si>
     <t>Parameter Estimator must be integrated into the GUI before the next meeting with Arne and Babett</t>
+  </si>
+  <si>
+    <t>Create GTK Prototype</t>
+  </si>
+  <si>
+    <t>Investigate if Mono compiles the Windows Forms GUI</t>
   </si>
 </sst>
 </file>
@@ -610,7 +616,7 @@
   <dimension ref="A1:H210"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F12:F14"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -746,7 +752,7 @@
     </row>
     <row r="7" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B7" s="11" t="s">
         <v>10</v>
@@ -754,8 +760,12 @@
       <c r="C7" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="D7" s="12"/>
-      <c r="E7" s="12"/>
+      <c r="D7" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="E7" s="15">
+        <v>44275</v>
+      </c>
       <c r="F7" s="12" t="s">
         <v>23</v>
       </c>
@@ -811,9 +821,15 @@
       <c r="H9" s="13"/>
     </row>
     <row r="10" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="10"/>
-      <c r="B10" s="11"/>
-      <c r="C10" s="12"/>
+      <c r="A10" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>28</v>
+      </c>
       <c r="D10" s="12"/>
       <c r="E10" s="12"/>
       <c r="F10" s="12"/>
@@ -822,10 +838,16 @@
       </c>
       <c r="H10" s="13"/>
     </row>
-    <row r="11" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="10"/>
-      <c r="B11" s="11"/>
-      <c r="C11" s="12"/>
+    <row r="11" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A11" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>29</v>
+      </c>
       <c r="D11" s="12"/>
       <c r="E11" s="12"/>
       <c r="F11" s="12"/>

</xml_diff>

<commit_message>
Added PSO and etc
</commit_message>
<xml_diff>
--- a/documents/development/Active Tasklist.xlsx
+++ b/documents/development/Active Tasklist.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20372"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23127"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62004BFE-CDC7-4D9E-A641-12D21E141EF5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5780F455-F4E7-4608-9B50-5DBE6068BF4C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{4FAFD036-DF6C-46F8-9D4B-2736D29CB41D}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14160" xr2:uid="{4FAFD036-DF6C-46F8-9D4B-2736D29CB41D}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="32">
   <si>
     <t>☒</t>
   </si>
@@ -111,6 +111,12 @@
   </si>
   <si>
     <t>Investigate if Mono compiles the Windows Forms GUI</t>
+  </si>
+  <si>
+    <t>Plotting function for PSO</t>
+  </si>
+  <si>
+    <t>Plotting experimental data in Form4</t>
   </si>
 </sst>
 </file>
@@ -300,7 +306,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Standard 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000030000000}"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -317,7 +323,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -616,17 +622,17 @@
   <dimension ref="A1:H210"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="3" max="3" width="31" customWidth="1"/>
-    <col min="5" max="5" width="13.140625" customWidth="1"/>
-    <col min="6" max="6" width="19.5703125" customWidth="1"/>
+    <col min="5" max="5" width="13.1796875" customWidth="1"/>
+    <col min="6" max="6" width="19.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
@@ -649,7 +655,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="26" x14ac:dyDescent="0.35">
       <c r="A2" s="8" t="s">
         <v>0</v>
       </c>
@@ -670,7 +676,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="26" x14ac:dyDescent="0.35">
       <c r="A3" s="8" t="s">
         <v>0</v>
       </c>
@@ -691,7 +697,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A4" s="8" t="s">
         <v>0</v>
       </c>
@@ -712,7 +718,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="26" x14ac:dyDescent="0.35">
       <c r="A5" s="14" t="s">
         <v>1</v>
       </c>
@@ -730,7 +736,7 @@
       </c>
       <c r="H5" s="13"/>
     </row>
-    <row r="6" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="26" x14ac:dyDescent="0.35">
       <c r="A6" s="14" t="s">
         <v>1</v>
       </c>
@@ -750,8 +756,8 @@
       </c>
       <c r="H6" s="13"/>
     </row>
-    <row r="7" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A7" s="14" t="s">
+    <row r="7" spans="1:8" ht="39" x14ac:dyDescent="0.35">
+      <c r="A7" s="16" t="s">
         <v>0</v>
       </c>
       <c r="B7" s="11" t="s">
@@ -774,7 +780,7 @@
       </c>
       <c r="H7" s="13"/>
     </row>
-    <row r="8" spans="1:8" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="39" x14ac:dyDescent="0.35">
       <c r="A8" s="16" t="s">
         <v>0</v>
       </c>
@@ -796,9 +802,9 @@
       </c>
       <c r="H8" s="13"/>
     </row>
-    <row r="9" spans="1:8" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="14" t="s">
-        <v>1</v>
+    <row r="9" spans="1:8" ht="65" x14ac:dyDescent="0.35">
+      <c r="A9" s="16" t="s">
+        <v>0</v>
       </c>
       <c r="B9" s="11" t="s">
         <v>8</v>
@@ -820,8 +826,8 @@
       </c>
       <c r="H9" s="13"/>
     </row>
-    <row r="10" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="10" t="s">
+    <row r="10" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A10" s="14" t="s">
         <v>1</v>
       </c>
       <c r="B10" s="11" t="s">
@@ -838,8 +844,8 @@
       </c>
       <c r="H10" s="13"/>
     </row>
-    <row r="11" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A11" s="10" t="s">
+    <row r="11" spans="1:8" ht="26" x14ac:dyDescent="0.35">
+      <c r="A11" s="14" t="s">
         <v>1</v>
       </c>
       <c r="B11" s="11" t="s">
@@ -856,31 +862,47 @@
       </c>
       <c r="H11" s="13"/>
     </row>
-    <row r="12" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="10"/>
-      <c r="B12" s="11"/>
-      <c r="C12" s="12"/>
+    <row r="12" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A12" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="12" t="s">
+        <v>30</v>
+      </c>
       <c r="D12" s="12"/>
-      <c r="E12" s="12"/>
+      <c r="E12" s="15">
+        <v>44279</v>
+      </c>
       <c r="F12" s="12"/>
       <c r="G12">
         <v>11</v>
       </c>
       <c r="H12" s="13"/>
     </row>
-    <row r="13" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="10"/>
-      <c r="B13" s="11"/>
-      <c r="C13" s="12"/>
+    <row r="13" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A13" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>31</v>
+      </c>
       <c r="D13" s="12"/>
-      <c r="E13" s="12"/>
+      <c r="E13" s="15">
+        <v>44279</v>
+      </c>
       <c r="F13" s="12"/>
       <c r="G13">
         <v>12</v>
       </c>
       <c r="H13" s="13"/>
     </row>
-    <row r="14" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A14" s="10"/>
       <c r="B14" s="11"/>
       <c r="C14" s="12"/>
@@ -892,7 +914,7 @@
       </c>
       <c r="H14" s="13"/>
     </row>
-    <row r="15" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A15" s="10"/>
       <c r="B15" s="11"/>
       <c r="C15" s="12"/>
@@ -904,7 +926,7 @@
       </c>
       <c r="H15" s="13"/>
     </row>
-    <row r="16" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A16" s="10"/>
       <c r="B16" s="11"/>
       <c r="C16" s="12"/>
@@ -916,7 +938,7 @@
       </c>
       <c r="H16" s="13"/>
     </row>
-    <row r="17" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A17" s="10"/>
       <c r="B17" s="11"/>
       <c r="C17" s="12"/>
@@ -928,7 +950,7 @@
       </c>
       <c r="H17" s="13"/>
     </row>
-    <row r="18" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A18" s="10"/>
       <c r="B18" s="11"/>
       <c r="C18" s="12"/>
@@ -940,7 +962,7 @@
       </c>
       <c r="H18" s="13"/>
     </row>
-    <row r="19" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A19" s="10"/>
       <c r="B19" s="11"/>
       <c r="C19" s="12"/>
@@ -950,7 +972,7 @@
       <c r="G19" s="13"/>
       <c r="H19" s="13"/>
     </row>
-    <row r="20" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A20" s="10"/>
       <c r="B20" s="11"/>
       <c r="C20" s="12"/>
@@ -960,7 +982,7 @@
       <c r="G20" s="13"/>
       <c r="H20" s="13"/>
     </row>
-    <row r="21" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A21" s="10"/>
       <c r="B21" s="11"/>
       <c r="C21" s="12"/>
@@ -970,7 +992,7 @@
       <c r="G21" s="13"/>
       <c r="H21" s="13"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A22" s="13"/>
       <c r="B22" s="13"/>
       <c r="C22" s="13"/>
@@ -980,7 +1002,7 @@
       <c r="G22" s="13"/>
       <c r="H22" s="13"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A23" s="13"/>
       <c r="B23" s="13"/>
       <c r="C23" s="13"/>
@@ -990,7 +1012,7 @@
       <c r="G23" s="13"/>
       <c r="H23" s="13"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A24" s="13"/>
       <c r="B24" s="13"/>
       <c r="C24" s="13"/>
@@ -1000,7 +1022,7 @@
       <c r="G24" s="13"/>
       <c r="H24" s="13"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A25" s="13"/>
       <c r="B25" s="13"/>
       <c r="C25" s="13"/>
@@ -1010,7 +1032,7 @@
       <c r="G25" s="13"/>
       <c r="H25" s="13"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A26" s="13"/>
       <c r="B26" s="13"/>
       <c r="C26" s="13"/>
@@ -1020,7 +1042,7 @@
       <c r="G26" s="13"/>
       <c r="H26" s="13"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A27" s="13"/>
       <c r="B27" s="13"/>
       <c r="C27" s="13"/>
@@ -1030,7 +1052,7 @@
       <c r="G27" s="13"/>
       <c r="H27" s="13"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A28" s="13"/>
       <c r="B28" s="13"/>
       <c r="C28" s="13"/>
@@ -1040,7 +1062,7 @@
       <c r="G28" s="13"/>
       <c r="H28" s="13"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A29" s="13"/>
       <c r="B29" s="13"/>
       <c r="C29" s="13"/>
@@ -1050,7 +1072,7 @@
       <c r="G29" s="13"/>
       <c r="H29" s="13"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A30" s="13"/>
       <c r="B30" s="13"/>
       <c r="C30" s="13"/>
@@ -1060,7 +1082,7 @@
       <c r="G30" s="13"/>
       <c r="H30" s="13"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A31" s="13"/>
       <c r="B31" s="13"/>
       <c r="C31" s="13"/>
@@ -1070,7 +1092,7 @@
       <c r="G31" s="13"/>
       <c r="H31" s="13"/>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A32" s="13"/>
       <c r="B32" s="13"/>
       <c r="C32" s="13"/>
@@ -1080,7 +1102,7 @@
       <c r="G32" s="13"/>
       <c r="H32" s="13"/>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A33" s="13"/>
       <c r="B33" s="13"/>
       <c r="C33" s="13"/>
@@ -1090,7 +1112,7 @@
       <c r="G33" s="13"/>
       <c r="H33" s="13"/>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A34" s="13"/>
       <c r="B34" s="13"/>
       <c r="C34" s="13"/>
@@ -1100,7 +1122,7 @@
       <c r="G34" s="13"/>
       <c r="H34" s="13"/>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A35" s="13"/>
       <c r="B35" s="13"/>
       <c r="C35" s="13"/>
@@ -1110,7 +1132,7 @@
       <c r="G35" s="13"/>
       <c r="H35" s="13"/>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A36" s="13"/>
       <c r="B36" s="13"/>
       <c r="C36" s="13"/>
@@ -1120,7 +1142,7 @@
       <c r="G36" s="13"/>
       <c r="H36" s="13"/>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A37" s="13"/>
       <c r="B37" s="13"/>
       <c r="C37" s="13"/>
@@ -1130,7 +1152,7 @@
       <c r="G37" s="13"/>
       <c r="H37" s="13"/>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A38" s="13"/>
       <c r="B38" s="13"/>
       <c r="C38" s="13"/>
@@ -1140,7 +1162,7 @@
       <c r="G38" s="13"/>
       <c r="H38" s="13"/>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A39" s="13"/>
       <c r="B39" s="13"/>
       <c r="C39" s="13"/>
@@ -1150,7 +1172,7 @@
       <c r="G39" s="13"/>
       <c r="H39" s="13"/>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A40" s="13"/>
       <c r="B40" s="13"/>
       <c r="C40" s="13"/>
@@ -1160,7 +1182,7 @@
       <c r="G40" s="13"/>
       <c r="H40" s="13"/>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A41" s="13"/>
       <c r="B41" s="13"/>
       <c r="C41" s="13"/>
@@ -1170,7 +1192,7 @@
       <c r="G41" s="13"/>
       <c r="H41" s="13"/>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A42" s="13"/>
       <c r="B42" s="13"/>
       <c r="C42" s="13"/>
@@ -1180,7 +1202,7 @@
       <c r="G42" s="13"/>
       <c r="H42" s="13"/>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A43" s="13"/>
       <c r="B43" s="13"/>
       <c r="C43" s="13"/>
@@ -1190,7 +1212,7 @@
       <c r="G43" s="13"/>
       <c r="H43" s="13"/>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A44" s="13"/>
       <c r="B44" s="13"/>
       <c r="C44" s="13"/>
@@ -1200,7 +1222,7 @@
       <c r="G44" s="13"/>
       <c r="H44" s="13"/>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A45" s="13"/>
       <c r="B45" s="13"/>
       <c r="C45" s="13"/>
@@ -1210,7 +1232,7 @@
       <c r="G45" s="13"/>
       <c r="H45" s="13"/>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A46" s="13"/>
       <c r="B46" s="13"/>
       <c r="C46" s="13"/>
@@ -1220,7 +1242,7 @@
       <c r="G46" s="13"/>
       <c r="H46" s="13"/>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A47" s="13"/>
       <c r="B47" s="13"/>
       <c r="C47" s="13"/>
@@ -1230,7 +1252,7 @@
       <c r="G47" s="13"/>
       <c r="H47" s="13"/>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A48" s="13"/>
       <c r="B48" s="13"/>
       <c r="C48" s="13"/>
@@ -1240,7 +1262,7 @@
       <c r="G48" s="13"/>
       <c r="H48" s="13"/>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A49" s="13"/>
       <c r="B49" s="13"/>
       <c r="C49" s="13"/>
@@ -1250,7 +1272,7 @@
       <c r="G49" s="13"/>
       <c r="H49" s="13"/>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A50" s="13"/>
       <c r="B50" s="13"/>
       <c r="C50" s="13"/>
@@ -1260,7 +1282,7 @@
       <c r="G50" s="13"/>
       <c r="H50" s="13"/>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A51" s="13"/>
       <c r="B51" s="13"/>
       <c r="C51" s="13"/>
@@ -1270,7 +1292,7 @@
       <c r="G51" s="13"/>
       <c r="H51" s="13"/>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A52" s="13"/>
       <c r="B52" s="13"/>
       <c r="C52" s="13"/>
@@ -1280,7 +1302,7 @@
       <c r="G52" s="13"/>
       <c r="H52" s="13"/>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A53" s="13"/>
       <c r="B53" s="13"/>
       <c r="C53" s="13"/>
@@ -1290,7 +1312,7 @@
       <c r="G53" s="13"/>
       <c r="H53" s="13"/>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A54" s="13"/>
       <c r="B54" s="13"/>
       <c r="C54" s="13"/>
@@ -1300,7 +1322,7 @@
       <c r="G54" s="13"/>
       <c r="H54" s="13"/>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A55" s="13"/>
       <c r="B55" s="13"/>
       <c r="C55" s="13"/>
@@ -1310,7 +1332,7 @@
       <c r="G55" s="13"/>
       <c r="H55" s="13"/>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A56" s="13"/>
       <c r="B56" s="13"/>
       <c r="C56" s="13"/>
@@ -1320,7 +1342,7 @@
       <c r="G56" s="13"/>
       <c r="H56" s="13"/>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A57" s="13"/>
       <c r="B57" s="13"/>
       <c r="C57" s="13"/>
@@ -1330,7 +1352,7 @@
       <c r="G57" s="13"/>
       <c r="H57" s="13"/>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A58" s="13"/>
       <c r="B58" s="13"/>
       <c r="C58" s="13"/>
@@ -1340,7 +1362,7 @@
       <c r="G58" s="13"/>
       <c r="H58" s="13"/>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A59" s="13"/>
       <c r="B59" s="13"/>
       <c r="C59" s="13"/>
@@ -1350,7 +1372,7 @@
       <c r="G59" s="13"/>
       <c r="H59" s="13"/>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A60" s="13"/>
       <c r="B60" s="13"/>
       <c r="C60" s="13"/>
@@ -1360,7 +1382,7 @@
       <c r="G60" s="13"/>
       <c r="H60" s="13"/>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A61" s="13"/>
       <c r="B61" s="13"/>
       <c r="C61" s="13"/>
@@ -1370,7 +1392,7 @@
       <c r="G61" s="13"/>
       <c r="H61" s="13"/>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A62" s="13"/>
       <c r="B62" s="13"/>
       <c r="C62" s="13"/>
@@ -1380,7 +1402,7 @@
       <c r="G62" s="13"/>
       <c r="H62" s="13"/>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A63" s="13"/>
       <c r="B63" s="13"/>
       <c r="C63" s="13"/>
@@ -1390,7 +1412,7 @@
       <c r="G63" s="13"/>
       <c r="H63" s="13"/>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A64" s="13"/>
       <c r="B64" s="13"/>
       <c r="C64" s="13"/>
@@ -1400,7 +1422,7 @@
       <c r="G64" s="13"/>
       <c r="H64" s="13"/>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A65" s="13"/>
       <c r="B65" s="13"/>
       <c r="C65" s="13"/>
@@ -1410,7 +1432,7 @@
       <c r="G65" s="13"/>
       <c r="H65" s="13"/>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A66" s="13"/>
       <c r="B66" s="13"/>
       <c r="C66" s="13"/>
@@ -1420,7 +1442,7 @@
       <c r="G66" s="13"/>
       <c r="H66" s="13"/>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A67" s="13"/>
       <c r="B67" s="13"/>
       <c r="C67" s="13"/>
@@ -1430,7 +1452,7 @@
       <c r="G67" s="13"/>
       <c r="H67" s="13"/>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A68" s="13"/>
       <c r="B68" s="13"/>
       <c r="C68" s="13"/>
@@ -1440,7 +1462,7 @@
       <c r="G68" s="13"/>
       <c r="H68" s="13"/>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A69" s="13"/>
       <c r="B69" s="13"/>
       <c r="C69" s="13"/>
@@ -1450,7 +1472,7 @@
       <c r="G69" s="13"/>
       <c r="H69" s="13"/>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A70" s="13"/>
       <c r="B70" s="13"/>
       <c r="C70" s="13"/>
@@ -1460,7 +1482,7 @@
       <c r="G70" s="13"/>
       <c r="H70" s="13"/>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A71" s="13"/>
       <c r="B71" s="13"/>
       <c r="C71" s="13"/>
@@ -1470,7 +1492,7 @@
       <c r="G71" s="13"/>
       <c r="H71" s="13"/>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A72" s="13"/>
       <c r="B72" s="13"/>
       <c r="C72" s="13"/>
@@ -1480,7 +1502,7 @@
       <c r="G72" s="13"/>
       <c r="H72" s="13"/>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A73" s="13"/>
       <c r="B73" s="13"/>
       <c r="C73" s="13"/>
@@ -1490,7 +1512,7 @@
       <c r="G73" s="13"/>
       <c r="H73" s="13"/>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A74" s="13"/>
       <c r="B74" s="13"/>
       <c r="C74" s="13"/>
@@ -1500,7 +1522,7 @@
       <c r="G74" s="13"/>
       <c r="H74" s="13"/>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A75" s="13"/>
       <c r="B75" s="13"/>
       <c r="C75" s="13"/>
@@ -1510,7 +1532,7 @@
       <c r="G75" s="13"/>
       <c r="H75" s="13"/>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A76" s="13"/>
       <c r="B76" s="13"/>
       <c r="C76" s="13"/>
@@ -1520,7 +1542,7 @@
       <c r="G76" s="13"/>
       <c r="H76" s="13"/>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A77" s="13"/>
       <c r="B77" s="13"/>
       <c r="C77" s="13"/>
@@ -1530,7 +1552,7 @@
       <c r="G77" s="13"/>
       <c r="H77" s="13"/>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A78" s="13"/>
       <c r="B78" s="13"/>
       <c r="C78" s="13"/>
@@ -1540,7 +1562,7 @@
       <c r="G78" s="13"/>
       <c r="H78" s="13"/>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A79" s="13"/>
       <c r="B79" s="13"/>
       <c r="C79" s="13"/>
@@ -1550,7 +1572,7 @@
       <c r="G79" s="13"/>
       <c r="H79" s="13"/>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A80" s="13"/>
       <c r="B80" s="13"/>
       <c r="C80" s="13"/>
@@ -1560,7 +1582,7 @@
       <c r="G80" s="13"/>
       <c r="H80" s="13"/>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A81" s="13"/>
       <c r="B81" s="13"/>
       <c r="C81" s="13"/>
@@ -1570,7 +1592,7 @@
       <c r="G81" s="13"/>
       <c r="H81" s="13"/>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A82" s="13"/>
       <c r="B82" s="13"/>
       <c r="C82" s="13"/>
@@ -1580,7 +1602,7 @@
       <c r="G82" s="13"/>
       <c r="H82" s="13"/>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A83" s="13"/>
       <c r="B83" s="13"/>
       <c r="C83" s="13"/>
@@ -1590,7 +1612,7 @@
       <c r="G83" s="13"/>
       <c r="H83" s="13"/>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A84" s="13"/>
       <c r="B84" s="13"/>
       <c r="C84" s="13"/>
@@ -1600,7 +1622,7 @@
       <c r="G84" s="13"/>
       <c r="H84" s="13"/>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A85" s="13"/>
       <c r="B85" s="13"/>
       <c r="C85" s="13"/>
@@ -1610,7 +1632,7 @@
       <c r="G85" s="13"/>
       <c r="H85" s="13"/>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A86" s="13"/>
       <c r="B86" s="13"/>
       <c r="C86" s="13"/>
@@ -1620,7 +1642,7 @@
       <c r="G86" s="13"/>
       <c r="H86" s="13"/>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A87" s="13"/>
       <c r="B87" s="13"/>
       <c r="C87" s="13"/>
@@ -1630,7 +1652,7 @@
       <c r="G87" s="13"/>
       <c r="H87" s="13"/>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A88" s="13"/>
       <c r="B88" s="13"/>
       <c r="C88" s="13"/>
@@ -1640,7 +1662,7 @@
       <c r="G88" s="13"/>
       <c r="H88" s="13"/>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A89" s="13"/>
       <c r="B89" s="13"/>
       <c r="C89" s="13"/>
@@ -1650,7 +1672,7 @@
       <c r="G89" s="13"/>
       <c r="H89" s="13"/>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A90" s="13"/>
       <c r="B90" s="13"/>
       <c r="C90" s="13"/>
@@ -1660,7 +1682,7 @@
       <c r="G90" s="13"/>
       <c r="H90" s="13"/>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A91" s="13"/>
       <c r="B91" s="13"/>
       <c r="C91" s="13"/>
@@ -1670,7 +1692,7 @@
       <c r="G91" s="13"/>
       <c r="H91" s="13"/>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A92" s="13"/>
       <c r="B92" s="13"/>
       <c r="C92" s="13"/>
@@ -1680,7 +1702,7 @@
       <c r="G92" s="13"/>
       <c r="H92" s="13"/>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A93" s="13"/>
       <c r="B93" s="13"/>
       <c r="C93" s="13"/>
@@ -1690,7 +1712,7 @@
       <c r="G93" s="13"/>
       <c r="H93" s="13"/>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A94" s="13"/>
       <c r="B94" s="13"/>
       <c r="C94" s="13"/>
@@ -1700,7 +1722,7 @@
       <c r="G94" s="13"/>
       <c r="H94" s="13"/>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A95" s="13"/>
       <c r="B95" s="13"/>
       <c r="C95" s="13"/>
@@ -1710,7 +1732,7 @@
       <c r="G95" s="13"/>
       <c r="H95" s="13"/>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A96" s="13"/>
       <c r="B96" s="13"/>
       <c r="C96" s="13"/>
@@ -1720,7 +1742,7 @@
       <c r="G96" s="13"/>
       <c r="H96" s="13"/>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A97" s="13"/>
       <c r="B97" s="13"/>
       <c r="C97" s="13"/>
@@ -1730,7 +1752,7 @@
       <c r="G97" s="13"/>
       <c r="H97" s="13"/>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A98" s="13"/>
       <c r="B98" s="13"/>
       <c r="C98" s="13"/>
@@ -1740,7 +1762,7 @@
       <c r="G98" s="13"/>
       <c r="H98" s="13"/>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A99" s="13"/>
       <c r="B99" s="13"/>
       <c r="C99" s="13"/>
@@ -1750,7 +1772,7 @@
       <c r="G99" s="13"/>
       <c r="H99" s="13"/>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A100" s="13"/>
       <c r="B100" s="13"/>
       <c r="C100" s="13"/>
@@ -1760,7 +1782,7 @@
       <c r="G100" s="13"/>
       <c r="H100" s="13"/>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A101" s="13"/>
       <c r="B101" s="13"/>
       <c r="C101" s="13"/>
@@ -1770,7 +1792,7 @@
       <c r="G101" s="13"/>
       <c r="H101" s="13"/>
     </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A102" s="13"/>
       <c r="B102" s="13"/>
       <c r="C102" s="13"/>
@@ -1780,7 +1802,7 @@
       <c r="G102" s="13"/>
       <c r="H102" s="13"/>
     </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A103" s="13"/>
       <c r="B103" s="13"/>
       <c r="C103" s="13"/>
@@ -1790,7 +1812,7 @@
       <c r="G103" s="13"/>
       <c r="H103" s="13"/>
     </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A104" s="13"/>
       <c r="B104" s="13"/>
       <c r="C104" s="13"/>
@@ -1800,7 +1822,7 @@
       <c r="G104" s="13"/>
       <c r="H104" s="13"/>
     </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A105" s="13"/>
       <c r="B105" s="13"/>
       <c r="C105" s="13"/>
@@ -1810,7 +1832,7 @@
       <c r="G105" s="13"/>
       <c r="H105" s="13"/>
     </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A106" s="13"/>
       <c r="B106" s="13"/>
       <c r="C106" s="13"/>
@@ -1820,7 +1842,7 @@
       <c r="G106" s="13"/>
       <c r="H106" s="13"/>
     </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A107" s="13"/>
       <c r="B107" s="13"/>
       <c r="C107" s="13"/>
@@ -1830,7 +1852,7 @@
       <c r="G107" s="13"/>
       <c r="H107" s="13"/>
     </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A108" s="13"/>
       <c r="B108" s="13"/>
       <c r="C108" s="13"/>
@@ -1840,7 +1862,7 @@
       <c r="G108" s="13"/>
       <c r="H108" s="13"/>
     </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A109" s="13"/>
       <c r="B109" s="13"/>
       <c r="C109" s="13"/>
@@ -1850,7 +1872,7 @@
       <c r="G109" s="13"/>
       <c r="H109" s="13"/>
     </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A110" s="13"/>
       <c r="B110" s="13"/>
       <c r="C110" s="13"/>
@@ -1860,7 +1882,7 @@
       <c r="G110" s="13"/>
       <c r="H110" s="13"/>
     </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A111" s="13"/>
       <c r="B111" s="13"/>
       <c r="C111" s="13"/>
@@ -1870,7 +1892,7 @@
       <c r="G111" s="13"/>
       <c r="H111" s="13"/>
     </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A112" s="13"/>
       <c r="B112" s="13"/>
       <c r="C112" s="13"/>
@@ -1880,7 +1902,7 @@
       <c r="G112" s="13"/>
       <c r="H112" s="13"/>
     </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A113" s="13"/>
       <c r="B113" s="13"/>
       <c r="C113" s="13"/>
@@ -1890,7 +1912,7 @@
       <c r="G113" s="13"/>
       <c r="H113" s="13"/>
     </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A114" s="13"/>
       <c r="B114" s="13"/>
       <c r="C114" s="13"/>
@@ -1900,7 +1922,7 @@
       <c r="G114" s="13"/>
       <c r="H114" s="13"/>
     </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A115" s="13"/>
       <c r="B115" s="13"/>
       <c r="C115" s="13"/>
@@ -1910,7 +1932,7 @@
       <c r="G115" s="13"/>
       <c r="H115" s="13"/>
     </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A116" s="13"/>
       <c r="B116" s="13"/>
       <c r="C116" s="13"/>
@@ -1920,7 +1942,7 @@
       <c r="G116" s="13"/>
       <c r="H116" s="13"/>
     </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A117" s="13"/>
       <c r="B117" s="13"/>
       <c r="C117" s="13"/>
@@ -1930,7 +1952,7 @@
       <c r="G117" s="13"/>
       <c r="H117" s="13"/>
     </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A118" s="13"/>
       <c r="B118" s="13"/>
       <c r="C118" s="13"/>
@@ -1940,7 +1962,7 @@
       <c r="G118" s="13"/>
       <c r="H118" s="13"/>
     </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A119" s="13"/>
       <c r="B119" s="13"/>
       <c r="C119" s="13"/>
@@ -1950,7 +1972,7 @@
       <c r="G119" s="13"/>
       <c r="H119" s="13"/>
     </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A120" s="13"/>
       <c r="B120" s="13"/>
       <c r="C120" s="13"/>
@@ -1960,7 +1982,7 @@
       <c r="G120" s="13"/>
       <c r="H120" s="13"/>
     </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A121" s="13"/>
       <c r="B121" s="13"/>
       <c r="C121" s="13"/>
@@ -1970,7 +1992,7 @@
       <c r="G121" s="13"/>
       <c r="H121" s="13"/>
     </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A122" s="13"/>
       <c r="B122" s="13"/>
       <c r="C122" s="13"/>
@@ -1980,7 +2002,7 @@
       <c r="G122" s="13"/>
       <c r="H122" s="13"/>
     </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A123" s="13"/>
       <c r="B123" s="13"/>
       <c r="C123" s="13"/>
@@ -1990,7 +2012,7 @@
       <c r="G123" s="13"/>
       <c r="H123" s="13"/>
     </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A124" s="13"/>
       <c r="B124" s="13"/>
       <c r="C124" s="13"/>
@@ -2000,7 +2022,7 @@
       <c r="G124" s="13"/>
       <c r="H124" s="13"/>
     </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A125" s="13"/>
       <c r="B125" s="13"/>
       <c r="C125" s="13"/>
@@ -2010,7 +2032,7 @@
       <c r="G125" s="13"/>
       <c r="H125" s="13"/>
     </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A126" s="13"/>
       <c r="B126" s="13"/>
       <c r="C126" s="13"/>
@@ -2020,7 +2042,7 @@
       <c r="G126" s="13"/>
       <c r="H126" s="13"/>
     </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A127" s="13"/>
       <c r="B127" s="13"/>
       <c r="C127" s="13"/>
@@ -2030,7 +2052,7 @@
       <c r="G127" s="13"/>
       <c r="H127" s="13"/>
     </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A128" s="13"/>
       <c r="B128" s="13"/>
       <c r="C128" s="13"/>
@@ -2040,7 +2062,7 @@
       <c r="G128" s="13"/>
       <c r="H128" s="13"/>
     </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A129" s="13"/>
       <c r="B129" s="13"/>
       <c r="C129" s="13"/>
@@ -2050,7 +2072,7 @@
       <c r="G129" s="13"/>
       <c r="H129" s="13"/>
     </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A130" s="13"/>
       <c r="B130" s="13"/>
       <c r="C130" s="13"/>
@@ -2060,7 +2082,7 @@
       <c r="G130" s="13"/>
       <c r="H130" s="13"/>
     </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A131" s="13"/>
       <c r="B131" s="13"/>
       <c r="C131" s="13"/>
@@ -2070,7 +2092,7 @@
       <c r="G131" s="13"/>
       <c r="H131" s="13"/>
     </row>
-    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A132" s="13"/>
       <c r="B132" s="13"/>
       <c r="C132" s="13"/>
@@ -2080,7 +2102,7 @@
       <c r="G132" s="13"/>
       <c r="H132" s="13"/>
     </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A133" s="13"/>
       <c r="B133" s="13"/>
       <c r="C133" s="13"/>
@@ -2090,7 +2112,7 @@
       <c r="G133" s="13"/>
       <c r="H133" s="13"/>
     </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A134" s="13"/>
       <c r="B134" s="13"/>
       <c r="C134" s="13"/>
@@ -2100,7 +2122,7 @@
       <c r="G134" s="13"/>
       <c r="H134" s="13"/>
     </row>
-    <row r="135" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A135" s="13"/>
       <c r="B135" s="13"/>
       <c r="C135" s="13"/>
@@ -2110,7 +2132,7 @@
       <c r="G135" s="13"/>
       <c r="H135" s="13"/>
     </row>
-    <row r="136" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A136" s="13"/>
       <c r="B136" s="13"/>
       <c r="C136" s="13"/>
@@ -2120,7 +2142,7 @@
       <c r="G136" s="13"/>
       <c r="H136" s="13"/>
     </row>
-    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A137" s="13"/>
       <c r="B137" s="13"/>
       <c r="C137" s="13"/>
@@ -2130,7 +2152,7 @@
       <c r="G137" s="13"/>
       <c r="H137" s="13"/>
     </row>
-    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A138" s="13"/>
       <c r="B138" s="13"/>
       <c r="C138" s="13"/>
@@ -2140,7 +2162,7 @@
       <c r="G138" s="13"/>
       <c r="H138" s="13"/>
     </row>
-    <row r="139" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A139" s="13"/>
       <c r="B139" s="13"/>
       <c r="C139" s="13"/>
@@ -2150,7 +2172,7 @@
       <c r="G139" s="13"/>
       <c r="H139" s="13"/>
     </row>
-    <row r="140" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A140" s="13"/>
       <c r="B140" s="13"/>
       <c r="C140" s="13"/>
@@ -2160,7 +2182,7 @@
       <c r="G140" s="13"/>
       <c r="H140" s="13"/>
     </row>
-    <row r="141" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A141" s="13"/>
       <c r="B141" s="13"/>
       <c r="C141" s="13"/>
@@ -2170,7 +2192,7 @@
       <c r="G141" s="13"/>
       <c r="H141" s="13"/>
     </row>
-    <row r="142" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A142" s="13"/>
       <c r="B142" s="13"/>
       <c r="C142" s="13"/>
@@ -2180,7 +2202,7 @@
       <c r="G142" s="13"/>
       <c r="H142" s="13"/>
     </row>
-    <row r="143" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A143" s="13"/>
       <c r="B143" s="13"/>
       <c r="C143" s="13"/>
@@ -2190,7 +2212,7 @@
       <c r="G143" s="13"/>
       <c r="H143" s="13"/>
     </row>
-    <row r="144" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A144" s="13"/>
       <c r="B144" s="13"/>
       <c r="C144" s="13"/>
@@ -2200,7 +2222,7 @@
       <c r="G144" s="13"/>
       <c r="H144" s="13"/>
     </row>
-    <row r="145" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A145" s="13"/>
       <c r="B145" s="13"/>
       <c r="C145" s="13"/>
@@ -2210,7 +2232,7 @@
       <c r="G145" s="13"/>
       <c r="H145" s="13"/>
     </row>
-    <row r="146" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A146" s="13"/>
       <c r="B146" s="13"/>
       <c r="C146" s="13"/>
@@ -2220,7 +2242,7 @@
       <c r="G146" s="13"/>
       <c r="H146" s="13"/>
     </row>
-    <row r="147" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A147" s="13"/>
       <c r="B147" s="13"/>
       <c r="C147" s="13"/>
@@ -2230,7 +2252,7 @@
       <c r="G147" s="13"/>
       <c r="H147" s="13"/>
     </row>
-    <row r="148" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A148" s="13"/>
       <c r="B148" s="13"/>
       <c r="C148" s="13"/>
@@ -2240,7 +2262,7 @@
       <c r="G148" s="13"/>
       <c r="H148" s="13"/>
     </row>
-    <row r="149" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A149" s="13"/>
       <c r="B149" s="13"/>
       <c r="C149" s="13"/>
@@ -2250,7 +2272,7 @@
       <c r="G149" s="13"/>
       <c r="H149" s="13"/>
     </row>
-    <row r="150" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A150" s="13"/>
       <c r="B150" s="13"/>
       <c r="C150" s="13"/>
@@ -2260,7 +2282,7 @@
       <c r="G150" s="13"/>
       <c r="H150" s="13"/>
     </row>
-    <row r="151" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A151" s="13"/>
       <c r="B151" s="13"/>
       <c r="C151" s="13"/>
@@ -2270,7 +2292,7 @@
       <c r="G151" s="13"/>
       <c r="H151" s="13"/>
     </row>
-    <row r="152" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A152" s="13"/>
       <c r="B152" s="13"/>
       <c r="C152" s="13"/>
@@ -2280,7 +2302,7 @@
       <c r="G152" s="13"/>
       <c r="H152" s="13"/>
     </row>
-    <row r="153" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A153" s="13"/>
       <c r="B153" s="13"/>
       <c r="C153" s="13"/>
@@ -2290,7 +2312,7 @@
       <c r="G153" s="13"/>
       <c r="H153" s="13"/>
     </row>
-    <row r="154" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A154" s="13"/>
       <c r="B154" s="13"/>
       <c r="C154" s="13"/>
@@ -2300,7 +2322,7 @@
       <c r="G154" s="13"/>
       <c r="H154" s="13"/>
     </row>
-    <row r="155" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A155" s="13"/>
       <c r="B155" s="13"/>
       <c r="C155" s="13"/>
@@ -2310,7 +2332,7 @@
       <c r="G155" s="13"/>
       <c r="H155" s="13"/>
     </row>
-    <row r="156" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A156" s="13"/>
       <c r="B156" s="13"/>
       <c r="C156" s="13"/>
@@ -2320,7 +2342,7 @@
       <c r="G156" s="13"/>
       <c r="H156" s="13"/>
     </row>
-    <row r="157" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A157" s="13"/>
       <c r="B157" s="13"/>
       <c r="C157" s="13"/>
@@ -2330,7 +2352,7 @@
       <c r="G157" s="13"/>
       <c r="H157" s="13"/>
     </row>
-    <row r="158" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A158" s="13"/>
       <c r="B158" s="13"/>
       <c r="C158" s="13"/>
@@ -2340,7 +2362,7 @@
       <c r="G158" s="13"/>
       <c r="H158" s="13"/>
     </row>
-    <row r="159" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A159" s="13"/>
       <c r="B159" s="13"/>
       <c r="C159" s="13"/>
@@ -2350,7 +2372,7 @@
       <c r="G159" s="13"/>
       <c r="H159" s="13"/>
     </row>
-    <row r="160" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A160" s="13"/>
       <c r="B160" s="13"/>
       <c r="C160" s="13"/>
@@ -2360,7 +2382,7 @@
       <c r="G160" s="13"/>
       <c r="H160" s="13"/>
     </row>
-    <row r="161" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A161" s="13"/>
       <c r="B161" s="13"/>
       <c r="C161" s="13"/>
@@ -2370,7 +2392,7 @@
       <c r="G161" s="13"/>
       <c r="H161" s="13"/>
     </row>
-    <row r="162" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A162" s="13"/>
       <c r="B162" s="13"/>
       <c r="C162" s="13"/>
@@ -2380,7 +2402,7 @@
       <c r="G162" s="13"/>
       <c r="H162" s="13"/>
     </row>
-    <row r="163" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A163" s="13"/>
       <c r="B163" s="13"/>
       <c r="C163" s="13"/>
@@ -2390,7 +2412,7 @@
       <c r="G163" s="13"/>
       <c r="H163" s="13"/>
     </row>
-    <row r="164" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A164" s="13"/>
       <c r="B164" s="13"/>
       <c r="C164" s="13"/>
@@ -2400,7 +2422,7 @@
       <c r="G164" s="13"/>
       <c r="H164" s="13"/>
     </row>
-    <row r="165" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A165" s="13"/>
       <c r="B165" s="13"/>
       <c r="C165" s="13"/>
@@ -2410,7 +2432,7 @@
       <c r="G165" s="13"/>
       <c r="H165" s="13"/>
     </row>
-    <row r="166" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A166" s="13"/>
       <c r="B166" s="13"/>
       <c r="C166" s="13"/>
@@ -2420,7 +2442,7 @@
       <c r="G166" s="13"/>
       <c r="H166" s="13"/>
     </row>
-    <row r="167" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A167" s="13"/>
       <c r="B167" s="13"/>
       <c r="C167" s="13"/>
@@ -2430,7 +2452,7 @@
       <c r="G167" s="13"/>
       <c r="H167" s="13"/>
     </row>
-    <row r="168" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A168" s="13"/>
       <c r="B168" s="13"/>
       <c r="C168" s="13"/>
@@ -2440,7 +2462,7 @@
       <c r="G168" s="13"/>
       <c r="H168" s="13"/>
     </row>
-    <row r="169" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A169" s="13"/>
       <c r="B169" s="13"/>
       <c r="C169" s="13"/>
@@ -2450,7 +2472,7 @@
       <c r="G169" s="13"/>
       <c r="H169" s="13"/>
     </row>
-    <row r="170" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A170" s="13"/>
       <c r="B170" s="13"/>
       <c r="C170" s="13"/>
@@ -2460,7 +2482,7 @@
       <c r="G170" s="13"/>
       <c r="H170" s="13"/>
     </row>
-    <row r="171" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A171" s="13"/>
       <c r="B171" s="13"/>
       <c r="C171" s="13"/>
@@ -2470,7 +2492,7 @@
       <c r="G171" s="13"/>
       <c r="H171" s="13"/>
     </row>
-    <row r="172" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A172" s="13"/>
       <c r="B172" s="13"/>
       <c r="C172" s="13"/>
@@ -2480,7 +2502,7 @@
       <c r="G172" s="13"/>
       <c r="H172" s="13"/>
     </row>
-    <row r="173" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A173" s="13"/>
       <c r="B173" s="13"/>
       <c r="C173" s="13"/>
@@ -2490,7 +2512,7 @@
       <c r="G173" s="13"/>
       <c r="H173" s="13"/>
     </row>
-    <row r="174" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A174" s="13"/>
       <c r="B174" s="13"/>
       <c r="C174" s="13"/>
@@ -2500,7 +2522,7 @@
       <c r="G174" s="13"/>
       <c r="H174" s="13"/>
     </row>
-    <row r="175" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A175" s="13"/>
       <c r="B175" s="13"/>
       <c r="C175" s="13"/>
@@ -2510,7 +2532,7 @@
       <c r="G175" s="13"/>
       <c r="H175" s="13"/>
     </row>
-    <row r="176" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A176" s="13"/>
       <c r="B176" s="13"/>
       <c r="C176" s="13"/>
@@ -2520,7 +2542,7 @@
       <c r="G176" s="13"/>
       <c r="H176" s="13"/>
     </row>
-    <row r="177" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A177" s="13"/>
       <c r="B177" s="13"/>
       <c r="C177" s="13"/>
@@ -2530,7 +2552,7 @@
       <c r="G177" s="13"/>
       <c r="H177" s="13"/>
     </row>
-    <row r="178" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A178" s="13"/>
       <c r="B178" s="13"/>
       <c r="C178" s="13"/>
@@ -2540,7 +2562,7 @@
       <c r="G178" s="13"/>
       <c r="H178" s="13"/>
     </row>
-    <row r="179" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A179" s="13"/>
       <c r="B179" s="13"/>
       <c r="C179" s="13"/>
@@ -2550,7 +2572,7 @@
       <c r="G179" s="13"/>
       <c r="H179" s="13"/>
     </row>
-    <row r="180" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A180" s="13"/>
       <c r="B180" s="13"/>
       <c r="C180" s="13"/>
@@ -2560,7 +2582,7 @@
       <c r="G180" s="13"/>
       <c r="H180" s="13"/>
     </row>
-    <row r="181" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A181" s="13"/>
       <c r="B181" s="13"/>
       <c r="C181" s="13"/>
@@ -2570,7 +2592,7 @@
       <c r="G181" s="13"/>
       <c r="H181" s="13"/>
     </row>
-    <row r="182" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A182" s="13"/>
       <c r="B182" s="13"/>
       <c r="C182" s="13"/>
@@ -2580,7 +2602,7 @@
       <c r="G182" s="13"/>
       <c r="H182" s="13"/>
     </row>
-    <row r="183" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A183" s="13"/>
       <c r="B183" s="13"/>
       <c r="C183" s="13"/>
@@ -2590,7 +2612,7 @@
       <c r="G183" s="13"/>
       <c r="H183" s="13"/>
     </row>
-    <row r="184" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A184" s="13"/>
       <c r="B184" s="13"/>
       <c r="C184" s="13"/>
@@ -2600,7 +2622,7 @@
       <c r="G184" s="13"/>
       <c r="H184" s="13"/>
     </row>
-    <row r="185" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A185" s="13"/>
       <c r="B185" s="13"/>
       <c r="C185" s="13"/>
@@ -2610,7 +2632,7 @@
       <c r="G185" s="13"/>
       <c r="H185" s="13"/>
     </row>
-    <row r="186" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A186" s="13"/>
       <c r="B186" s="13"/>
       <c r="C186" s="13"/>
@@ -2620,7 +2642,7 @@
       <c r="G186" s="13"/>
       <c r="H186" s="13"/>
     </row>
-    <row r="187" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A187" s="13"/>
       <c r="B187" s="13"/>
       <c r="C187" s="13"/>
@@ -2630,7 +2652,7 @@
       <c r="G187" s="13"/>
       <c r="H187" s="13"/>
     </row>
-    <row r="188" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A188" s="13"/>
       <c r="B188" s="13"/>
       <c r="C188" s="13"/>
@@ -2640,7 +2662,7 @@
       <c r="G188" s="13"/>
       <c r="H188" s="13"/>
     </row>
-    <row r="189" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A189" s="13"/>
       <c r="B189" s="13"/>
       <c r="C189" s="13"/>
@@ -2650,7 +2672,7 @@
       <c r="G189" s="13"/>
       <c r="H189" s="13"/>
     </row>
-    <row r="190" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A190" s="13"/>
       <c r="B190" s="13"/>
       <c r="C190" s="13"/>
@@ -2660,7 +2682,7 @@
       <c r="G190" s="13"/>
       <c r="H190" s="13"/>
     </row>
-    <row r="191" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A191" s="13"/>
       <c r="B191" s="13"/>
       <c r="C191" s="13"/>
@@ -2670,7 +2692,7 @@
       <c r="G191" s="13"/>
       <c r="H191" s="13"/>
     </row>
-    <row r="192" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A192" s="13"/>
       <c r="B192" s="13"/>
       <c r="C192" s="13"/>
@@ -2680,7 +2702,7 @@
       <c r="G192" s="13"/>
       <c r="H192" s="13"/>
     </row>
-    <row r="193" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A193" s="13"/>
       <c r="B193" s="13"/>
       <c r="C193" s="13"/>
@@ -2690,7 +2712,7 @@
       <c r="G193" s="13"/>
       <c r="H193" s="13"/>
     </row>
-    <row r="194" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A194" s="13"/>
       <c r="B194" s="13"/>
       <c r="C194" s="13"/>
@@ -2700,7 +2722,7 @@
       <c r="G194" s="13"/>
       <c r="H194" s="13"/>
     </row>
-    <row r="195" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A195" s="13"/>
       <c r="B195" s="13"/>
       <c r="C195" s="13"/>
@@ -2710,7 +2732,7 @@
       <c r="G195" s="13"/>
       <c r="H195" s="13"/>
     </row>
-    <row r="196" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A196" s="13"/>
       <c r="B196" s="13"/>
       <c r="C196" s="13"/>
@@ -2720,7 +2742,7 @@
       <c r="G196" s="13"/>
       <c r="H196" s="13"/>
     </row>
-    <row r="197" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A197" s="13"/>
       <c r="B197" s="13"/>
       <c r="C197" s="13"/>
@@ -2730,7 +2752,7 @@
       <c r="G197" s="13"/>
       <c r="H197" s="13"/>
     </row>
-    <row r="198" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A198" s="13"/>
       <c r="B198" s="13"/>
       <c r="C198" s="13"/>
@@ -2740,7 +2762,7 @@
       <c r="G198" s="13"/>
       <c r="H198" s="13"/>
     </row>
-    <row r="199" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A199" s="13"/>
       <c r="B199" s="13"/>
       <c r="C199" s="13"/>
@@ -2750,7 +2772,7 @@
       <c r="G199" s="13"/>
       <c r="H199" s="13"/>
     </row>
-    <row r="200" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A200" s="13"/>
       <c r="B200" s="13"/>
       <c r="C200" s="13"/>
@@ -2760,7 +2782,7 @@
       <c r="G200" s="13"/>
       <c r="H200" s="13"/>
     </row>
-    <row r="201" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A201" s="13"/>
       <c r="B201" s="13"/>
       <c r="C201" s="13"/>
@@ -2770,7 +2792,7 @@
       <c r="G201" s="13"/>
       <c r="H201" s="13"/>
     </row>
-    <row r="202" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A202" s="13"/>
       <c r="B202" s="13"/>
       <c r="C202" s="13"/>
@@ -2780,7 +2802,7 @@
       <c r="G202" s="13"/>
       <c r="H202" s="13"/>
     </row>
-    <row r="203" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A203" s="13"/>
       <c r="B203" s="13"/>
       <c r="C203" s="13"/>
@@ -2790,7 +2812,7 @@
       <c r="G203" s="13"/>
       <c r="H203" s="13"/>
     </row>
-    <row r="204" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A204" s="13"/>
       <c r="B204" s="13"/>
       <c r="C204" s="13"/>
@@ -2800,7 +2822,7 @@
       <c r="G204" s="13"/>
       <c r="H204" s="13"/>
     </row>
-    <row r="205" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A205" s="13"/>
       <c r="B205" s="13"/>
       <c r="C205" s="13"/>
@@ -2810,7 +2832,7 @@
       <c r="G205" s="13"/>
       <c r="H205" s="13"/>
     </row>
-    <row r="206" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A206" s="13"/>
       <c r="B206" s="13"/>
       <c r="C206" s="13"/>
@@ -2820,7 +2842,7 @@
       <c r="G206" s="13"/>
       <c r="H206" s="13"/>
     </row>
-    <row r="207" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A207" s="13"/>
       <c r="B207" s="13"/>
       <c r="C207" s="13"/>
@@ -2830,7 +2852,7 @@
       <c r="G207" s="13"/>
       <c r="H207" s="13"/>
     </row>
-    <row r="208" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A208" s="13"/>
       <c r="B208" s="13"/>
       <c r="C208" s="13"/>
@@ -2840,7 +2862,7 @@
       <c r="G208" s="13"/>
       <c r="H208" s="13"/>
     </row>
-    <row r="209" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A209" s="13"/>
       <c r="B209" s="13"/>
       <c r="C209" s="13"/>
@@ -2850,7 +2872,7 @@
       <c r="G209" s="13"/>
       <c r="H209" s="13"/>
     </row>
-    <row r="210" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A210" s="13"/>
       <c r="B210" s="13"/>
       <c r="C210" s="13"/>
@@ -2901,9 +2923,9 @@
       <selection activeCell="C2" sqref="C2:C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -2914,7 +2936,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -2925,7 +2947,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -2936,7 +2958,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -2944,7 +2966,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>6</v>
       </c>

</xml_diff>

<commit_message>
Form8 completed, samples added, documentation improved
</commit_message>
<xml_diff>
--- a/documents/development/Active Tasklist.xlsx
+++ b/documents/development/Active Tasklist.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23901"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41B3C625-302D-4EA9-BA61-DF87AEACAA44}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDF66254-6074-4B77-AD94-E14AD5494368}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14160" xr2:uid="{4FAFD036-DF6C-46F8-9D4B-2736D29CB41D}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="32">
   <si>
     <t>☒</t>
   </si>
@@ -184,7 +184,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -224,6 +224,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -308,9 +314,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="14" fontId="7" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
@@ -318,6 +321,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="7" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -638,7 +644,7 @@
   <dimension ref="A1:H210"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14:G18"/>
+      <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -735,9 +741,7 @@
       </c>
     </row>
     <row r="5" spans="1:8" ht="26" x14ac:dyDescent="0.35">
-      <c r="A5" s="14" t="s">
-        <v>1</v>
-      </c>
+      <c r="A5" s="17"/>
       <c r="B5" s="11" t="s">
         <v>9</v>
       </c>
@@ -753,8 +757,8 @@
       <c r="H5" s="13"/>
     </row>
     <row r="6" spans="1:8" ht="26" x14ac:dyDescent="0.35">
-      <c r="A6" s="14" t="s">
-        <v>1</v>
+      <c r="A6" s="15" t="s">
+        <v>0</v>
       </c>
       <c r="B6" s="11" t="s">
         <v>10</v>
@@ -773,7 +777,7 @@
       <c r="H6" s="13"/>
     </row>
     <row r="7" spans="1:8" ht="39" x14ac:dyDescent="0.35">
-      <c r="A7" s="16" t="s">
+      <c r="A7" s="15" t="s">
         <v>0</v>
       </c>
       <c r="B7" s="11" t="s">
@@ -785,7 +789,7 @@
       <c r="D7" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="E7" s="15">
+      <c r="E7" s="14">
         <v>44275</v>
       </c>
       <c r="F7" s="12" t="s">
@@ -797,7 +801,7 @@
       <c r="H7" s="13"/>
     </row>
     <row r="8" spans="1:8" ht="39" x14ac:dyDescent="0.35">
-      <c r="A8" s="16" t="s">
+      <c r="A8" s="15" t="s">
         <v>0</v>
       </c>
       <c r="B8" s="11" t="s">
@@ -809,7 +813,7 @@
       <c r="D8" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="E8" s="15">
+      <c r="E8" s="14">
         <v>44275</v>
       </c>
       <c r="F8" s="12"/>
@@ -819,7 +823,7 @@
       <c r="H8" s="13"/>
     </row>
     <row r="9" spans="1:8" ht="65" x14ac:dyDescent="0.35">
-      <c r="A9" s="16" t="s">
+      <c r="A9" s="15" t="s">
         <v>0</v>
       </c>
       <c r="B9" s="11" t="s">
@@ -831,7 +835,7 @@
       <c r="D9" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E9" s="15">
+      <c r="E9" s="14">
         <v>44279</v>
       </c>
       <c r="F9" s="12" t="s">
@@ -843,7 +847,7 @@
       <c r="H9" s="13"/>
     </row>
     <row r="10" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A10" s="16" t="s">
+      <c r="A10" s="15" t="s">
         <v>0</v>
       </c>
       <c r="B10" s="11" t="s">
@@ -861,7 +865,7 @@
       <c r="H10" s="13"/>
     </row>
     <row r="11" spans="1:8" ht="26" x14ac:dyDescent="0.35">
-      <c r="A11" s="17" t="s">
+      <c r="A11" s="16" t="s">
         <v>1</v>
       </c>
       <c r="B11" s="11" t="s">
@@ -879,7 +883,7 @@
       <c r="H11" s="13"/>
     </row>
     <row r="12" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A12" s="16" t="s">
+      <c r="A12" s="15" t="s">
         <v>0</v>
       </c>
       <c r="B12" s="11" t="s">
@@ -889,7 +893,7 @@
         <v>30</v>
       </c>
       <c r="D12" s="12"/>
-      <c r="E12" s="15">
+      <c r="E12" s="14">
         <v>44279</v>
       </c>
       <c r="F12" s="12"/>
@@ -899,7 +903,7 @@
       <c r="H12" s="13"/>
     </row>
     <row r="13" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A13" s="16" t="s">
+      <c r="A13" s="15" t="s">
         <v>0</v>
       </c>
       <c r="B13" s="11" t="s">
@@ -909,7 +913,7 @@
         <v>31</v>
       </c>
       <c r="D13" s="12"/>
-      <c r="E13" s="15">
+      <c r="E13" s="14">
         <v>44279</v>
       </c>
       <c r="F13" s="12"/>

</xml_diff>

<commit_message>
Fixed cale of experimental data graph in relation to other satapoints in seird ode gui widget
</commit_message>
<xml_diff>
--- a/documents/development/Active Tasklist.xlsx
+++ b/documents/development/Active Tasklist.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="62">
   <si>
     <t xml:space="preserve">Status</t>
   </si>
@@ -213,11 +213,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
+  <numFmts count="5">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
-    <numFmt numFmtId="166" formatCode="dd/mm/yy"/>
-    <numFmt numFmtId="167" formatCode="mm/dd/yy"/>
+    <numFmt numFmtId="165" formatCode="DD/MM/YYYY"/>
+    <numFmt numFmtId="166" formatCode="DD/MM/YY"/>
+    <numFmt numFmtId="167" formatCode="DD/MM/YY"/>
+    <numFmt numFmtId="168" formatCode="MM/DD/YY"/>
   </numFmts>
   <fonts count="9">
     <font>
@@ -399,13 +400,13 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="2" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="3" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="2" borderId="2" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -417,19 +418,19 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="4" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="2" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="3" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="2" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="3" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="6" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="2" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="3" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="5" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="2" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="3" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="6" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -449,18 +450,22 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="6" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="2" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="3" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="5" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="167" fontId="6" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="3" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -546,21 +551,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:H210"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C33" activeCellId="0" sqref="C33"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C29" activeCellId="0" sqref="C29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.91015625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="10.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="82.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="10.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="13.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="19.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="10.91"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -977,9 +985,9 @@
       </c>
       <c r="H20" s="9"/>
     </row>
-    <row r="21" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="55.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="13" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="B21" s="7" t="s">
         <v>11</v>
@@ -987,8 +995,12 @@
       <c r="C21" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
+      <c r="D21" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E21" s="14" t="n">
+        <v>44349</v>
+      </c>
       <c r="F21" s="5" t="s">
         <v>41</v>
       </c>
@@ -1001,16 +1013,16 @@
       <c r="A22" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="B22" s="14" t="s">
+      <c r="B22" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="C22" s="14" t="s">
+      <c r="C22" s="15" t="s">
         <v>42</v>
       </c>
       <c r="D22" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="E22" s="15" t="s">
+      <c r="E22" s="16" t="s">
         <v>43</v>
       </c>
       <c r="F22" s="9" t="s">
@@ -1022,13 +1034,13 @@
       <c r="H22" s="9"/>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="14" t="s">
+      <c r="A23" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="B23" s="14" t="s">
+      <c r="B23" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="C23" s="14" t="s">
+      <c r="C23" s="15" t="s">
         <v>45</v>
       </c>
       <c r="D23" s="9" t="s">
@@ -1044,13 +1056,13 @@
       <c r="H23" s="9"/>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="14" t="s">
+      <c r="A24" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="B24" s="14" t="s">
+      <c r="B24" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="C24" s="14" t="s">
+      <c r="C24" s="15" t="s">
         <v>48</v>
       </c>
       <c r="D24" s="9"/>
@@ -1064,13 +1076,13 @@
       <c r="H24" s="9"/>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="14" t="s">
+      <c r="A25" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="B25" s="14" t="s">
+      <c r="B25" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="C25" s="14" t="s">
+      <c r="C25" s="15" t="s">
         <v>50</v>
       </c>
       <c r="D25" s="9"/>
@@ -1084,13 +1096,13 @@
       <c r="H25" s="9"/>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="14" t="s">
+      <c r="A26" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="B26" s="14" t="s">
+      <c r="B26" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="C26" s="14" t="s">
+      <c r="C26" s="15" t="s">
         <v>52</v>
       </c>
       <c r="D26" s="9"/>
@@ -1104,13 +1116,13 @@
       <c r="H26" s="9"/>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="14" t="s">
+      <c r="A27" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="B27" s="14" t="s">
+      <c r="B27" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="C27" s="14" t="s">
+      <c r="C27" s="15" t="s">
         <v>54</v>
       </c>
       <c r="D27" s="9"/>
@@ -1124,13 +1136,13 @@
       <c r="H27" s="9"/>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="14" t="s">
+      <c r="A28" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="B28" s="14" t="s">
+      <c r="B28" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="C28" s="14" t="s">
+      <c r="C28" s="15" t="s">
         <v>56</v>
       </c>
       <c r="D28" s="9"/>
@@ -1144,7 +1156,7 @@
       <c r="H28" s="9"/>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="14" t="s">
+      <c r="A29" s="15" t="s">
         <v>25</v>
       </c>
       <c r="B29" s="9" t="s">
@@ -1164,7 +1176,7 @@
       <c r="H29" s="9"/>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="14"/>
+      <c r="A30" s="15"/>
       <c r="B30" s="9"/>
       <c r="C30" s="9"/>
       <c r="D30" s="9"/>
@@ -1176,7 +1188,7 @@
       <c r="H30" s="9"/>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="14"/>
+      <c r="A31" s="15"/>
       <c r="B31" s="9"/>
       <c r="C31" s="9"/>
       <c r="D31" s="9"/>
@@ -3057,7 +3069,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -3067,7 +3079,10 @@
       <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.91015625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="10.91"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -3087,7 +3102,7 @@
       <c r="B2" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="C2" s="17" t="s">
         <v>7</v>
       </c>
     </row>
@@ -3095,7 +3110,7 @@
       <c r="A3" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="18" t="s">
         <v>11</v>
       </c>
       <c r="C3" s="3" t="s">

</xml_diff>

<commit_message>
- Updated Tasklist and .gitignore
</commit_message>
<xml_diff>
--- a/documents/development/Active Tasklist.xlsx
+++ b/documents/development/Active Tasklist.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="63">
   <si>
     <t xml:space="preserve">Status</t>
   </si>
@@ -201,6 +201,9 @@
   </si>
   <si>
     <t xml:space="preserve">During an optimization procedure, a lot of information is relayed to the user (see summary_of_estimation.txt). Ideally, this information would be shown during the optimization to the user (just like in the command line)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Create All-in-One Executable</t>
   </si>
   <si>
     <t xml:space="preserve">Developers</t>
@@ -213,12 +216,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="5">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="DD/MM/YYYY"/>
-    <numFmt numFmtId="166" formatCode="DD/MM/YY"/>
-    <numFmt numFmtId="167" formatCode="DD/MM/YY"/>
-    <numFmt numFmtId="168" formatCode="MM/DD/YY"/>
+    <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
+    <numFmt numFmtId="166" formatCode="dd/mm/yy"/>
+    <numFmt numFmtId="167" formatCode="mm/dd/yy"/>
   </numFmts>
   <fonts count="9">
     <font>
@@ -400,13 +402,13 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="3" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="6" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="2" borderId="2" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -418,19 +420,19 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="4" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="3" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="6" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="3" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="6" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="6" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="3" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="6" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="5" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="3" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="6" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="6" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -450,22 +452,26 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="6" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="3" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="6" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="5" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="6" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="3" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="6" fillId="5" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="6" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="167" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -551,24 +557,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:H210"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C29" activeCellId="0" sqref="C29"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A6" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F21" activeCellId="0" sqref="F21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.89453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="10.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.47"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="82.08"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="10.91"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="13.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="18.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="13.19"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="19.54"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="10.91"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -985,11 +990,11 @@
       </c>
       <c r="H20" s="9"/>
     </row>
-    <row r="21" customFormat="false" ht="55.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="13" t="s">
+    <row r="21" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="B21" s="7" t="s">
+      <c r="B21" s="14" t="s">
         <v>11</v>
       </c>
       <c r="C21" s="5" t="s">
@@ -998,10 +1003,10 @@
       <c r="D21" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E21" s="14" t="n">
+      <c r="E21" s="12" t="n">
         <v>44349</v>
       </c>
-      <c r="F21" s="5" t="s">
+      <c r="F21" s="15" t="s">
         <v>41</v>
       </c>
       <c r="G21" s="0" t="n">
@@ -1013,16 +1018,16 @@
       <c r="A22" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="B22" s="15" t="s">
+      <c r="B22" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="C22" s="15" t="s">
+      <c r="C22" s="16" t="s">
         <v>42</v>
       </c>
       <c r="D22" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="E22" s="16" t="s">
+      <c r="E22" s="17" t="s">
         <v>43</v>
       </c>
       <c r="F22" s="9" t="s">
@@ -1034,13 +1039,13 @@
       <c r="H22" s="9"/>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="15" t="s">
+      <c r="A23" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="B23" s="15" t="s">
+      <c r="B23" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="C23" s="15" t="s">
+      <c r="C23" s="16" t="s">
         <v>45</v>
       </c>
       <c r="D23" s="9" t="s">
@@ -1056,13 +1061,13 @@
       <c r="H23" s="9"/>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="15" t="s">
+      <c r="A24" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="B24" s="15" t="s">
+      <c r="B24" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="C24" s="15" t="s">
+      <c r="C24" s="16" t="s">
         <v>48</v>
       </c>
       <c r="D24" s="9"/>
@@ -1076,13 +1081,13 @@
       <c r="H24" s="9"/>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="15" t="s">
+      <c r="A25" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="B25" s="15" t="s">
+      <c r="B25" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="C25" s="15" t="s">
+      <c r="C25" s="16" t="s">
         <v>50</v>
       </c>
       <c r="D25" s="9"/>
@@ -1096,13 +1101,13 @@
       <c r="H25" s="9"/>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="15" t="s">
+      <c r="A26" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="B26" s="15" t="s">
+      <c r="B26" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="C26" s="15" t="s">
+      <c r="C26" s="16" t="s">
         <v>52</v>
       </c>
       <c r="D26" s="9"/>
@@ -1116,13 +1121,13 @@
       <c r="H26" s="9"/>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="15" t="s">
+      <c r="A27" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="B27" s="15" t="s">
+      <c r="B27" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="C27" s="15" t="s">
+      <c r="C27" s="16" t="s">
         <v>54</v>
       </c>
       <c r="D27" s="9"/>
@@ -1136,13 +1141,13 @@
       <c r="H27" s="9"/>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="15" t="s">
+      <c r="A28" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="B28" s="15" t="s">
+      <c r="B28" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="C28" s="15" t="s">
+      <c r="C28" s="16" t="s">
         <v>56</v>
       </c>
       <c r="D28" s="9"/>
@@ -1156,10 +1161,10 @@
       <c r="H28" s="9"/>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="15" t="s">
+      <c r="A29" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="B29" s="9" t="s">
+      <c r="B29" s="16" t="s">
         <v>11</v>
       </c>
       <c r="C29" s="9" t="s">
@@ -1176,10 +1181,18 @@
       <c r="H29" s="9"/>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="15"/>
-      <c r="B30" s="9"/>
-      <c r="C30" s="9"/>
-      <c r="D30" s="9"/>
+      <c r="A30" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="B30" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="C30" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="D30" s="9" t="s">
+        <v>30</v>
+      </c>
       <c r="E30" s="9"/>
       <c r="F30" s="9"/>
       <c r="G30" s="0" t="n">
@@ -1188,7 +1201,7 @@
       <c r="H30" s="9"/>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="15"/>
+      <c r="A31" s="16"/>
       <c r="B31" s="9"/>
       <c r="C31" s="9"/>
       <c r="D31" s="9"/>
@@ -3041,26 +3054,26 @@
     </row>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation allowBlank="true" error="Invalid developer name" errorTitle="Wrong" operator="equal" prompt="Select an available developer from the list" promptTitle="Developers" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D1" type="none">
+    <dataValidation allowBlank="true" error="Invalid developer name" errorStyle="stop" errorTitle="Wrong" operator="equal" prompt="Select an available developer from the list" promptTitle="Developers" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D1" type="none">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" prompt="Decide if task is open or completed" promptTitle="Task Status" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="A2:A31" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" prompt="Decide if task is open or completed" promptTitle="Task Status" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="A2:A31" type="list">
       <formula1>Tabelle2!$C$2:$C$3</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" error="Invalid priority entered" errorTitle="Invalid priority" operator="equal" prompt="Priority of the task" promptTitle="Priority" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="B2:B25" type="list">
+    <dataValidation allowBlank="true" error="Invalid priority entered" errorStyle="stop" errorTitle="Invalid priority" operator="equal" prompt="Priority of the task" promptTitle="Priority" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="B2:B25" type="list">
       <formula1>Tabelle2!$B$2:$B$4</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" error="Invalid developer name" errorTitle="Wrong" operator="equal" prompt="Select an available developer from the list" promptTitle="Developers" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D2:D43" type="list">
+    <dataValidation allowBlank="true" error="Invalid developer name" errorStyle="stop" errorTitle="Wrong" operator="equal" prompt="Select an available developer from the list" promptTitle="Developers" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D2:D43" type="list">
       <formula1>Tabelle2!$A$2:$A$5</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -3069,7 +3082,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -3079,14 +3092,11 @@
       <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="10.91"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="10.89453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B1" s="0" t="s">
         <v>1</v>
@@ -3102,7 +3112,7 @@
       <c r="B2" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="17" t="s">
+      <c r="C2" s="18" t="s">
         <v>7</v>
       </c>
     </row>
@@ -3110,7 +3120,7 @@
       <c r="A3" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="B3" s="18" t="s">
+      <c r="B3" s="19" t="s">
         <v>11</v>
       </c>
       <c r="C3" s="3" t="s">
@@ -3132,13 +3142,13 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>

<commit_message>
Added preliminary Editor class and other smaller changes
</commit_message>
<xml_diff>
--- a/documents/development/Active Tasklist.xlsx
+++ b/documents/development/Active Tasklist.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="65">
   <si>
     <t xml:space="preserve">Status</t>
   </si>
@@ -204,6 +204,12 @@
   </si>
   <si>
     <t xml:space="preserve">Create All-in-One Executable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Create Editor Widget and call it from SEIRDPDE_EDITOR class</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Create Editor to arbitrarily draw initial conditions</t>
   </si>
   <si>
     <t xml:space="preserve">Developers</t>
@@ -218,9 +224,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
-    <numFmt numFmtId="166" formatCode="dd/mm/yy"/>
-    <numFmt numFmtId="167" formatCode="mm/dd/yy"/>
+    <numFmt numFmtId="165" formatCode="DD/MM/YYYY"/>
+    <numFmt numFmtId="166" formatCode="DD/MM/YY"/>
+    <numFmt numFmtId="167" formatCode="MM/DD/YY"/>
   </numFmts>
   <fonts count="9">
     <font>
@@ -408,7 +414,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="6" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="8" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="2" borderId="2" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -420,19 +426,19 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="4" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="6" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="8" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="6" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="8" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="6" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="6" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="8" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="5" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="6" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="8" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="6" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -452,7 +458,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="6" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="6" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="8" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="5" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -464,7 +470,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="6" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="8" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -557,23 +563,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:H210"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A6" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F21" activeCellId="0" sqref="F21"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D12" activeCellId="0" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.89453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.47"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="82.08"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="18.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="13.19"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="19.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="10.89"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1062,7 +1070,7 @@
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="16" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="B24" s="16" t="s">
         <v>8</v>
@@ -1070,7 +1078,9 @@
       <c r="C24" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="D24" s="9"/>
+      <c r="D24" s="9" t="s">
+        <v>30</v>
+      </c>
       <c r="E24" s="9"/>
       <c r="F24" s="9" t="s">
         <v>49</v>
@@ -1201,12 +1211,22 @@
       <c r="H30" s="9"/>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="16"/>
-      <c r="B31" s="9"/>
-      <c r="C31" s="9"/>
-      <c r="D31" s="9"/>
+      <c r="A31" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="B31" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C31" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="D31" s="9" t="s">
+        <v>46</v>
+      </c>
       <c r="E31" s="9"/>
-      <c r="F31" s="9"/>
+      <c r="F31" s="9" t="s">
+        <v>62</v>
+      </c>
       <c r="G31" s="0" t="n">
         <v>30</v>
       </c>
@@ -3054,26 +3074,26 @@
     </row>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation allowBlank="true" error="Invalid developer name" errorStyle="stop" errorTitle="Wrong" operator="equal" prompt="Select an available developer from the list" promptTitle="Developers" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D1" type="none">
+    <dataValidation allowBlank="true" error="Invalid developer name" errorTitle="Wrong" operator="equal" prompt="Select an available developer from the list" promptTitle="Developers" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D1" type="none">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" prompt="Decide if task is open or completed" promptTitle="Task Status" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="A2:A31" type="list">
+    <dataValidation allowBlank="true" operator="equal" prompt="Decide if task is open or completed" promptTitle="Task Status" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="A2:A31" type="list">
       <formula1>Tabelle2!$C$2:$C$3</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" error="Invalid priority entered" errorStyle="stop" errorTitle="Invalid priority" operator="equal" prompt="Priority of the task" promptTitle="Priority" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="B2:B25" type="list">
+    <dataValidation allowBlank="true" error="Invalid priority entered" errorTitle="Invalid priority" operator="equal" prompt="Priority of the task" promptTitle="Priority" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="B2:B25" type="list">
       <formula1>Tabelle2!$B$2:$B$4</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" error="Invalid developer name" errorStyle="stop" errorTitle="Wrong" operator="equal" prompt="Select an available developer from the list" promptTitle="Developers" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D2:D43" type="list">
+    <dataValidation allowBlank="true" error="Invalid developer name" errorTitle="Wrong" operator="equal" prompt="Select an available developer from the list" promptTitle="Developers" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D2:D43" type="list">
       <formula1>Tabelle2!$A$2:$A$5</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -3082,7 +3102,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -3092,11 +3112,14 @@
       <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.89453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="10.89"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B1" s="0" t="s">
         <v>1</v>
@@ -3142,13 +3165,13 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.7875" bottom="0.7875" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>

<commit_message>
Added ability to load greyscale images into GUI and convert these images into initial conditions
</commit_message>
<xml_diff>
--- a/documents/development/Active Tasklist.xlsx
+++ b/documents/development/Active Tasklist.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="67">
   <si>
     <t xml:space="preserve">Status</t>
   </si>
@@ -210,6 +210,12 @@
   </si>
   <si>
     <t xml:space="preserve">Create Editor to arbitrarily draw initial conditions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Create ability to load arbitrary images and convert them into square initial values for the PDE solver</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13/07/2021</t>
   </si>
   <si>
     <t xml:space="preserve">Developers</t>
@@ -408,13 +414,13 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="8" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="11" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="2" borderId="2" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -426,19 +432,19 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="4" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="8" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="11" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="8" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="11" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="6" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="8" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="11" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="5" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="8" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="11" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="6" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -458,7 +464,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="6" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="8" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="11" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="5" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -470,7 +476,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="8" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="11" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -479,6 +485,10 @@
     </xf>
     <xf numFmtId="167" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="9" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -569,8 +579,8 @@
   </sheetPr>
   <dimension ref="A1:H210"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D12" activeCellId="0" sqref="D12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C16" activeCellId="0" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1047,7 +1057,7 @@
       <c r="H22" s="9"/>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="16" t="s">
+      <c r="A23" s="18" t="s">
         <v>7</v>
       </c>
       <c r="B23" s="16" t="s">
@@ -1069,7 +1079,7 @@
       <c r="H23" s="9"/>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="16" t="s">
+      <c r="A24" s="18" t="s">
         <v>7</v>
       </c>
       <c r="B24" s="16" t="s">
@@ -1115,7 +1125,7 @@
         <v>25</v>
       </c>
       <c r="B26" s="16" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C26" s="16" t="s">
         <v>52</v>
@@ -1135,7 +1145,7 @@
         <v>25</v>
       </c>
       <c r="B27" s="16" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C27" s="16" t="s">
         <v>54</v>
@@ -1175,9 +1185,9 @@
         <v>25</v>
       </c>
       <c r="B29" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="C29" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C29" s="16" t="s">
         <v>58</v>
       </c>
       <c r="D29" s="9"/>
@@ -1197,7 +1207,7 @@
       <c r="B30" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="C30" s="9" t="s">
+      <c r="C30" s="16" t="s">
         <v>60</v>
       </c>
       <c r="D30" s="9" t="s">
@@ -1214,10 +1224,10 @@
       <c r="A31" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="B31" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="C31" s="9" t="s">
+      <c r="B31" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="C31" s="16" t="s">
         <v>61</v>
       </c>
       <c r="D31" s="9" t="s">
@@ -1233,11 +1243,21 @@
       <c r="H31" s="9"/>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="9"/>
-      <c r="B32" s="9"/>
-      <c r="C32" s="9"/>
-      <c r="D32" s="9"/>
-      <c r="E32" s="9"/>
+      <c r="A32" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="B32" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="C32" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="D32" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E32" s="9" t="s">
+        <v>64</v>
+      </c>
       <c r="F32" s="9"/>
       <c r="G32" s="0" t="n">
         <v>31</v>
@@ -1245,8 +1265,12 @@
       <c r="H32" s="9"/>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="9"/>
-      <c r="B33" s="9"/>
+      <c r="A33" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="B33" s="16" t="s">
+        <v>14</v>
+      </c>
       <c r="C33" s="9"/>
       <c r="D33" s="9"/>
       <c r="E33" s="9"/>
@@ -1257,8 +1281,12 @@
       <c r="H33" s="9"/>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="9"/>
-      <c r="B34" s="9"/>
+      <c r="A34" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="B34" s="16" t="s">
+        <v>14</v>
+      </c>
       <c r="C34" s="9"/>
       <c r="D34" s="9"/>
       <c r="E34" s="9"/>
@@ -1269,8 +1297,12 @@
       <c r="H34" s="9"/>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="9"/>
-      <c r="B35" s="9"/>
+      <c r="A35" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="B35" s="16" t="s">
+        <v>14</v>
+      </c>
       <c r="C35" s="9"/>
       <c r="D35" s="9"/>
       <c r="E35" s="9"/>
@@ -1281,8 +1313,12 @@
       <c r="H35" s="9"/>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="9"/>
-      <c r="B36" s="9"/>
+      <c r="A36" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="B36" s="16" t="s">
+        <v>14</v>
+      </c>
       <c r="C36" s="9"/>
       <c r="D36" s="9"/>
       <c r="E36" s="9"/>
@@ -1293,8 +1329,12 @@
       <c r="H36" s="9"/>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="9"/>
-      <c r="B37" s="9"/>
+      <c r="A37" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="B37" s="16" t="s">
+        <v>14</v>
+      </c>
       <c r="C37" s="9"/>
       <c r="D37" s="9"/>
       <c r="E37" s="9"/>
@@ -1305,8 +1345,12 @@
       <c r="H37" s="9"/>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="9"/>
-      <c r="B38" s="9"/>
+      <c r="A38" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="B38" s="16" t="s">
+        <v>14</v>
+      </c>
       <c r="C38" s="9"/>
       <c r="D38" s="9"/>
       <c r="E38" s="9"/>
@@ -1317,8 +1361,12 @@
       <c r="H38" s="9"/>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="9"/>
-      <c r="B39" s="9"/>
+      <c r="A39" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="B39" s="16" t="s">
+        <v>14</v>
+      </c>
       <c r="C39" s="9"/>
       <c r="D39" s="9"/>
       <c r="E39" s="9"/>
@@ -1329,8 +1377,12 @@
       <c r="H39" s="9"/>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="9"/>
-      <c r="B40" s="9"/>
+      <c r="A40" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="B40" s="16" t="s">
+        <v>14</v>
+      </c>
       <c r="C40" s="9"/>
       <c r="D40" s="9"/>
       <c r="E40" s="9"/>
@@ -1341,8 +1393,12 @@
       <c r="H40" s="9"/>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="9"/>
-      <c r="B41" s="9"/>
+      <c r="A41" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="B41" s="16" t="s">
+        <v>14</v>
+      </c>
       <c r="C41" s="9"/>
       <c r="D41" s="9"/>
       <c r="E41" s="9"/>
@@ -1353,8 +1409,12 @@
       <c r="H41" s="9"/>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="9"/>
-      <c r="B42" s="9"/>
+      <c r="A42" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="B42" s="16" t="s">
+        <v>14</v>
+      </c>
       <c r="C42" s="9"/>
       <c r="D42" s="9"/>
       <c r="E42" s="9"/>
@@ -1365,8 +1425,12 @@
       <c r="H42" s="9"/>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="9"/>
-      <c r="B43" s="9"/>
+      <c r="A43" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="B43" s="16" t="s">
+        <v>14</v>
+      </c>
       <c r="C43" s="9"/>
       <c r="D43" s="9"/>
       <c r="E43" s="9"/>
@@ -3078,11 +3142,11 @@
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" prompt="Decide if task is open or completed" promptTitle="Task Status" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="A2:A31" type="list">
+    <dataValidation allowBlank="true" operator="equal" prompt="Decide if task is open or completed" promptTitle="Task Status" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="A2:A43" type="list">
       <formula1>Tabelle2!$C$2:$C$3</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" error="Invalid priority entered" errorTitle="Invalid priority" operator="equal" prompt="Priority of the task" promptTitle="Priority" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="B2:B25" type="list">
+    <dataValidation allowBlank="true" error="Invalid priority entered" errorTitle="Invalid priority" operator="equal" prompt="Priority of the task" promptTitle="Priority" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="B2:B43" type="list">
       <formula1>Tabelle2!$B$2:$B$4</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -3119,7 +3183,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B1" s="0" t="s">
         <v>1</v>
@@ -3135,7 +3199,7 @@
       <c r="B2" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="18" t="s">
+      <c r="C2" s="19" t="s">
         <v>7</v>
       </c>
     </row>
@@ -3143,7 +3207,7 @@
       <c r="A3" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="B3" s="19" t="s">
+      <c r="B3" s="20" t="s">
         <v>11</v>
       </c>
       <c r="C3" s="3" t="s">
@@ -3165,7 +3229,7 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>